<commit_message>
edit csv_editor.py to make not erase .csv file, and remove generated files from git
</commit_message>
<xml_diff>
--- a/exceldata/Excel Plants Papa.xlsx
+++ b/exceldata/Excel Plants Papa.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="653">
   <si>
     <t>name</t>
   </si>
@@ -1981,6 +1981,9 @@
   </si>
   <si>
     <t>Identique à celeri branche, à la différence que celui-ci est vivace</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -2301,6 +2304,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2315,9 +2321,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2607,10 +2610,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AA1" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="AJ143" sqref="AJ143"/>
+      <selection pane="bottomLeft" activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2635,7 +2638,7 @@
     <col min="20" max="20" width="21" style="6" customWidth="1"/>
     <col min="21" max="21" width="18.109375" style="6" customWidth="1"/>
     <col min="22" max="22" width="18.33203125" style="6" customWidth="1"/>
-    <col min="23" max="23" width="6.44140625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" style="7" customWidth="1"/>
     <col min="24" max="24" width="10.88671875" style="3" customWidth="1"/>
     <col min="25" max="25" width="15.5546875" style="3" customWidth="1"/>
     <col min="26" max="26" width="21.109375" style="1" customWidth="1"/>
@@ -2664,32 +2667,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="28" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="28" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
       <c r="S1" s="32" t="s">
         <v>143</v>
       </c>
@@ -2697,57 +2700,57 @@
       <c r="U1" s="33"/>
       <c r="V1" s="33"/>
       <c r="W1" s="33"/>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="31" t="s">
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31" t="s">
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31" t="s">
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26" t="s">
         <v>447</v>
       </c>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31" t="s">
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26" t="s">
         <v>448</v>
       </c>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31" t="s">
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31" t="s">
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31" t="s">
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31" t="s">
+      <c r="AU1" s="26"/>
+      <c r="AV1" s="26"/>
+      <c r="AW1" s="26" t="s">
         <v>444</v>
       </c>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31" t="s">
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="26"/>
+      <c r="AZ1" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
+      <c r="BA1" s="26"/>
+      <c r="BB1" s="26"/>
     </row>
     <row r="2" spans="1:54" s="25" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
@@ -3429,6 +3432,9 @@
       <c r="V7" s="10">
         <v>44075</v>
       </c>
+      <c r="W7" s="7">
+        <v>1</v>
+      </c>
       <c r="X7" s="3">
         <v>5</v>
       </c>
@@ -3535,6 +3541,9 @@
       <c r="V8" s="10">
         <v>44089</v>
       </c>
+      <c r="W8" s="7">
+        <v>1</v>
+      </c>
       <c r="X8" s="3">
         <v>6</v>
       </c>
@@ -3641,6 +3650,9 @@
       <c r="V9" s="10">
         <v>44044</v>
       </c>
+      <c r="W9" s="7">
+        <v>1</v>
+      </c>
       <c r="X9" s="3">
         <v>7</v>
       </c>
@@ -3747,6 +3759,9 @@
       <c r="V10" s="10">
         <v>43997</v>
       </c>
+      <c r="W10" s="7">
+        <v>1</v>
+      </c>
       <c r="X10" s="3">
         <v>8</v>
       </c>
@@ -3853,6 +3868,9 @@
       <c r="V11" s="10">
         <v>43983</v>
       </c>
+      <c r="W11" s="7">
+        <v>1</v>
+      </c>
       <c r="X11" s="3">
         <v>9</v>
       </c>
@@ -3959,6 +3977,9 @@
       <c r="V12" s="10">
         <v>43983</v>
       </c>
+      <c r="W12" s="7">
+        <v>1</v>
+      </c>
       <c r="X12" s="3">
         <v>10</v>
       </c>
@@ -4049,6 +4070,9 @@
       <c r="V13" s="10">
         <v>43983</v>
       </c>
+      <c r="W13" s="7">
+        <v>1</v>
+      </c>
       <c r="X13" s="3">
         <v>11</v>
       </c>
@@ -4139,6 +4163,9 @@
       <c r="V14" s="10">
         <v>43997</v>
       </c>
+      <c r="W14" s="7">
+        <v>1</v>
+      </c>
       <c r="X14" s="3">
         <v>12</v>
       </c>
@@ -4229,6 +4256,9 @@
       <c r="V15" s="10">
         <v>43983</v>
       </c>
+      <c r="W15" s="7">
+        <v>1</v>
+      </c>
       <c r="X15" s="3">
         <v>13</v>
       </c>
@@ -4319,6 +4349,9 @@
       <c r="V16" s="10">
         <v>43936</v>
       </c>
+      <c r="W16" s="7">
+        <v>1</v>
+      </c>
       <c r="X16" s="3">
         <v>14</v>
       </c>
@@ -4409,6 +4442,9 @@
       <c r="V17" s="10">
         <v>43966</v>
       </c>
+      <c r="W17" s="7">
+        <v>1</v>
+      </c>
       <c r="X17" s="3">
         <v>15</v>
       </c>
@@ -4499,6 +4535,9 @@
       <c r="V18" s="10">
         <v>43983</v>
       </c>
+      <c r="W18" s="7">
+        <v>1</v>
+      </c>
       <c r="X18" s="3">
         <v>16</v>
       </c>
@@ -4589,6 +4628,9 @@
       <c r="V19" s="10">
         <v>43983</v>
       </c>
+      <c r="W19" s="7">
+        <v>1</v>
+      </c>
       <c r="X19" s="3">
         <v>17</v>
       </c>
@@ -4679,6 +4721,9 @@
       <c r="V20" s="10">
         <v>43983</v>
       </c>
+      <c r="W20" s="7">
+        <v>1</v>
+      </c>
       <c r="X20" s="3">
         <v>18</v>
       </c>
@@ -4769,6 +4814,9 @@
       <c r="V21" s="10">
         <v>43983</v>
       </c>
+      <c r="W21" s="7">
+        <v>1</v>
+      </c>
       <c r="X21" s="3">
         <v>19</v>
       </c>
@@ -4859,6 +4907,9 @@
       <c r="V22" s="10">
         <v>43997</v>
       </c>
+      <c r="W22" s="7">
+        <v>1</v>
+      </c>
       <c r="X22" s="3">
         <v>20</v>
       </c>
@@ -4949,6 +5000,9 @@
       <c r="V23" s="10">
         <v>44058</v>
       </c>
+      <c r="W23" s="7">
+        <v>1</v>
+      </c>
       <c r="X23" s="3">
         <v>21</v>
       </c>
@@ -5039,6 +5093,9 @@
       <c r="V24" s="10">
         <v>44105</v>
       </c>
+      <c r="W24" s="7">
+        <v>1</v>
+      </c>
       <c r="X24" s="3">
         <v>22</v>
       </c>
@@ -5117,6 +5174,9 @@
       <c r="V25" s="10">
         <v>43936</v>
       </c>
+      <c r="W25" s="7">
+        <v>1</v>
+      </c>
       <c r="X25" s="3">
         <v>23</v>
       </c>
@@ -5195,6 +5255,9 @@
       <c r="V26" s="10">
         <v>44105</v>
       </c>
+      <c r="W26" s="7">
+        <v>1</v>
+      </c>
       <c r="X26" s="3">
         <v>24</v>
       </c>
@@ -5273,6 +5336,9 @@
       <c r="V27" s="10">
         <v>43966</v>
       </c>
+      <c r="W27" s="7">
+        <v>1</v>
+      </c>
       <c r="X27" s="3">
         <v>25</v>
       </c>
@@ -5351,6 +5417,9 @@
       <c r="V28" s="10">
         <v>43891</v>
       </c>
+      <c r="W28" s="7">
+        <v>1</v>
+      </c>
       <c r="X28" s="3">
         <v>26</v>
       </c>
@@ -5429,6 +5498,9 @@
       <c r="V29" s="10">
         <v>44075</v>
       </c>
+      <c r="W29" s="7">
+        <v>1</v>
+      </c>
       <c r="X29" s="3">
         <v>27</v>
       </c>
@@ -5507,6 +5579,9 @@
       <c r="V30" s="10">
         <v>44075</v>
       </c>
+      <c r="W30" s="7">
+        <v>1</v>
+      </c>
       <c r="X30" s="3">
         <v>28</v>
       </c>
@@ -5585,6 +5660,9 @@
       <c r="V31" s="10">
         <v>44075</v>
       </c>
+      <c r="W31" s="7">
+        <v>1</v>
+      </c>
       <c r="X31" s="3">
         <v>29</v>
       </c>
@@ -5663,6 +5741,9 @@
       <c r="V32" s="10">
         <v>44075</v>
       </c>
+      <c r="W32" s="7">
+        <v>1</v>
+      </c>
       <c r="X32" s="3">
         <v>30</v>
       </c>
@@ -5741,6 +5822,9 @@
       <c r="V33" s="10">
         <v>43936</v>
       </c>
+      <c r="W33" s="7">
+        <v>1</v>
+      </c>
       <c r="X33" s="3">
         <v>31</v>
       </c>
@@ -5819,6 +5903,9 @@
       <c r="V34" s="10">
         <v>43966</v>
       </c>
+      <c r="W34" s="7">
+        <v>1</v>
+      </c>
       <c r="X34" s="3">
         <v>32</v>
       </c>
@@ -5897,6 +5984,9 @@
       <c r="V35" s="10">
         <v>44119</v>
       </c>
+      <c r="W35" s="7">
+        <v>1</v>
+      </c>
       <c r="X35" s="3">
         <v>33</v>
       </c>
@@ -5975,6 +6065,9 @@
       <c r="V36" s="10">
         <v>44058</v>
       </c>
+      <c r="W36" s="7">
+        <v>1</v>
+      </c>
       <c r="X36" s="3">
         <v>34</v>
       </c>
@@ -6037,6 +6130,9 @@
       <c r="V37" s="10">
         <v>44089</v>
       </c>
+      <c r="W37" s="7">
+        <v>1</v>
+      </c>
       <c r="X37" s="3">
         <v>35</v>
       </c>
@@ -6099,6 +6195,9 @@
       <c r="V38" s="10">
         <v>43983</v>
       </c>
+      <c r="W38" s="7">
+        <v>1</v>
+      </c>
       <c r="X38" s="3">
         <v>36</v>
       </c>
@@ -6161,6 +6260,9 @@
       <c r="V39" s="10">
         <v>43983</v>
       </c>
+      <c r="W39" s="7">
+        <v>1</v>
+      </c>
       <c r="X39" s="3">
         <v>37</v>
       </c>
@@ -6223,6 +6325,9 @@
       <c r="V40" s="10">
         <v>43983</v>
       </c>
+      <c r="W40" s="7">
+        <v>1</v>
+      </c>
       <c r="X40" s="3">
         <v>38</v>
       </c>
@@ -7652,6 +7757,9 @@
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
+      <c r="AJ68" s="1" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="69" spans="14:36" x14ac:dyDescent="0.3">
       <c r="N69" s="2">
@@ -7799,6 +7907,9 @@
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
+      <c r="AJ71" s="1" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="72" spans="14:36" x14ac:dyDescent="0.3">
       <c r="N72" s="2">
@@ -8182,7 +8293,7 @@
         <v>77</v>
       </c>
       <c r="AF79" s="3">
-        <f>N24</f>
+        <f t="shared" ref="AF79:AF110" si="7">N24</f>
         <v>22</v>
       </c>
       <c r="AG79" s="1">
@@ -8232,7 +8343,7 @@
         <v>78</v>
       </c>
       <c r="AF80" s="3">
-        <f>N25</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="AG80" s="1">
@@ -8282,7 +8393,7 @@
         <v>79</v>
       </c>
       <c r="AF81" s="3">
-        <f>N26</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="AG81" s="1">
@@ -8330,7 +8441,7 @@
         <v>80</v>
       </c>
       <c r="AF82" s="3">
-        <f>N27</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="AG82" s="1">
@@ -8377,7 +8488,7 @@
         <v>81</v>
       </c>
       <c r="AF83" s="3">
-        <f>N28</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="AG83" s="1">
@@ -8424,7 +8535,7 @@
         <v>82</v>
       </c>
       <c r="AF84" s="3">
-        <f>N29</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="AG84" s="1">
@@ -8471,7 +8582,7 @@
         <v>83</v>
       </c>
       <c r="AF85" s="3">
-        <f>N30</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="AG85" s="1">
@@ -8518,7 +8629,7 @@
         <v>84</v>
       </c>
       <c r="AF86" s="3">
-        <f>N31</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="AG86" s="1">
@@ -8568,7 +8679,7 @@
         <v>85</v>
       </c>
       <c r="AF87" s="3">
-        <f>N32</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="AG87" s="1">
@@ -8618,7 +8729,7 @@
         <v>86</v>
       </c>
       <c r="AF88" s="3">
-        <f>N33</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="AG88" s="1">
@@ -8632,6 +8743,9 @@
         <f t="shared" si="6"/>
         <v>86</v>
       </c>
+      <c r="AJ88" s="1" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="89" spans="14:36" x14ac:dyDescent="0.3">
       <c r="N89" s="2">
@@ -8665,7 +8779,7 @@
         <v>87</v>
       </c>
       <c r="AF89" s="3">
-        <f>N34</f>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="AG89" s="1">
@@ -8715,7 +8829,7 @@
         <v>88</v>
       </c>
       <c r="AF90" s="3">
-        <f>N35</f>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="AG90" s="1">
@@ -8765,7 +8879,7 @@
         <v>89</v>
       </c>
       <c r="AF91" s="3">
-        <f>N36</f>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="AG91" s="1">
@@ -8815,7 +8929,7 @@
         <v>90</v>
       </c>
       <c r="AF92" s="3">
-        <f>N37</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="AG92" s="1">
@@ -8854,7 +8968,7 @@
         <v>94</v>
       </c>
       <c r="Y93" s="3">
-        <f t="shared" ref="Y93:Y99" si="7">N36</f>
+        <f t="shared" ref="Y93:Y99" si="8">N36</f>
         <v>34</v>
       </c>
       <c r="Z93" s="1">
@@ -8865,7 +8979,7 @@
         <v>91</v>
       </c>
       <c r="AF93" s="3">
-        <f>N38</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="AG93" s="1">
@@ -8904,7 +9018,7 @@
         <v>95</v>
       </c>
       <c r="Y94" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="Z94" s="1">
@@ -8915,7 +9029,7 @@
         <v>92</v>
       </c>
       <c r="AF94" s="3">
-        <f>N39</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="AG94" s="1">
@@ -8951,7 +9065,7 @@
         <v>96</v>
       </c>
       <c r="Y95" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="Z95" s="1">
@@ -8962,7 +9076,7 @@
         <v>93</v>
       </c>
       <c r="AF95" s="3">
-        <f>N40</f>
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
       <c r="AG95" s="1">
@@ -8998,7 +9112,7 @@
         <v>97</v>
       </c>
       <c r="Y96" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="Z96" s="1">
@@ -9009,7 +9123,7 @@
         <v>94</v>
       </c>
       <c r="AF96" s="3">
-        <f>N41</f>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
       <c r="AG96" s="1">
@@ -9048,7 +9162,7 @@
         <v>98</v>
       </c>
       <c r="Y97" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="Z97" s="1">
@@ -9059,7 +9173,7 @@
         <v>95</v>
       </c>
       <c r="AF97" s="3">
-        <f>N42</f>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="AG97" s="1">
@@ -9095,7 +9209,7 @@
         <v>99</v>
       </c>
       <c r="Y98" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
       <c r="Z98" s="1">
@@ -9106,7 +9220,7 @@
         <v>96</v>
       </c>
       <c r="AF98" s="3">
-        <f>N43</f>
+        <f t="shared" si="7"/>
         <v>41</v>
       </c>
       <c r="AG98" s="1">
@@ -9120,6 +9234,9 @@
         <f t="shared" si="6"/>
         <v>96</v>
       </c>
+      <c r="AJ98" s="1" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="99" spans="14:36" x14ac:dyDescent="0.3">
       <c r="N99" s="2">
@@ -9142,7 +9259,7 @@
         <v>100</v>
       </c>
       <c r="Y99" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="Z99" s="1">
@@ -9153,7 +9270,7 @@
         <v>97</v>
       </c>
       <c r="AF99" s="3">
-        <f>N44</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="AG99" s="1">
@@ -9189,7 +9306,7 @@
         <v>101</v>
       </c>
       <c r="Y100" s="3">
-        <f>N43</f>
+        <f t="shared" ref="Y100:Y131" si="9">N43</f>
         <v>41</v>
       </c>
       <c r="Z100" s="1">
@@ -9200,7 +9317,7 @@
         <v>98</v>
       </c>
       <c r="AF100" s="3">
-        <f>N45</f>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="AG100" s="1">
@@ -9239,7 +9356,7 @@
         <v>102</v>
       </c>
       <c r="Y101" s="3">
-        <f>N44</f>
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="Z101" s="1">
@@ -9250,7 +9367,7 @@
         <v>99</v>
       </c>
       <c r="AF101" s="3">
-        <f>N46</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="AG101" s="1">
@@ -9289,7 +9406,7 @@
         <v>103</v>
       </c>
       <c r="Y102" s="3">
-        <f>N45</f>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="Z102" s="1">
@@ -9300,7 +9417,7 @@
         <v>100</v>
       </c>
       <c r="AF102" s="3">
-        <f>N47</f>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="AG102" s="1">
@@ -9339,7 +9456,7 @@
         <v>104</v>
       </c>
       <c r="Y103" s="3">
-        <f>N46</f>
+        <f t="shared" si="9"/>
         <v>44</v>
       </c>
       <c r="Z103" s="1">
@@ -9350,7 +9467,7 @@
         <v>101</v>
       </c>
       <c r="AF103" s="3">
-        <f>N48</f>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="AG103" s="1">
@@ -9389,7 +9506,7 @@
         <v>105</v>
       </c>
       <c r="Y104" s="3">
-        <f>N47</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Z104" s="1">
@@ -9400,7 +9517,7 @@
         <v>102</v>
       </c>
       <c r="AF104" s="3">
-        <f>N49</f>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="AG104" s="1">
@@ -9439,7 +9556,7 @@
         <v>106</v>
       </c>
       <c r="Y105" s="3">
-        <f>N48</f>
+        <f t="shared" si="9"/>
         <v>46</v>
       </c>
       <c r="Z105" s="1">
@@ -9450,7 +9567,7 @@
         <v>103</v>
       </c>
       <c r="AF105" s="3">
-        <f>N50</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="AG105" s="1">
@@ -9489,7 +9606,7 @@
         <v>107</v>
       </c>
       <c r="Y106" s="3">
-        <f>N49</f>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="Z106" s="1">
@@ -9500,7 +9617,7 @@
         <v>104</v>
       </c>
       <c r="AF106" s="3">
-        <f>N51</f>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="AG106" s="1">
@@ -9539,7 +9656,7 @@
         <v>108</v>
       </c>
       <c r="Y107" s="3">
-        <f>N50</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="Z107" s="1">
@@ -9550,7 +9667,7 @@
         <v>105</v>
       </c>
       <c r="AF107" s="3">
-        <f>N52</f>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="AG107" s="1">
@@ -9561,7 +9678,7 @@
         <v>105</v>
       </c>
       <c r="AI107" s="3">
-        <f t="shared" ref="AI107:AI140" si="8">N107</f>
+        <f t="shared" ref="AI107:AI140" si="10">N107</f>
         <v>105</v>
       </c>
       <c r="AJ107" s="1" t="s">
@@ -9589,7 +9706,7 @@
         <v>109</v>
       </c>
       <c r="Y108" s="3">
-        <f>N51</f>
+        <f t="shared" si="9"/>
         <v>49</v>
       </c>
       <c r="Z108" s="1">
@@ -9600,7 +9717,7 @@
         <v>106</v>
       </c>
       <c r="AF108" s="3">
-        <f>N53</f>
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
       <c r="AG108" s="1">
@@ -9611,7 +9728,7 @@
         <v>106</v>
       </c>
       <c r="AI108" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>106</v>
       </c>
       <c r="AJ108" s="1" t="s">
@@ -9639,7 +9756,7 @@
         <v>110</v>
       </c>
       <c r="Y109" s="3">
-        <f>N52</f>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="Z109" s="1">
@@ -9650,7 +9767,7 @@
         <v>107</v>
       </c>
       <c r="AF109" s="3">
-        <f>N54</f>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="AG109" s="1">
@@ -9661,7 +9778,7 @@
         <v>107</v>
       </c>
       <c r="AI109" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>107</v>
       </c>
       <c r="AJ109" s="1" t="s">
@@ -9689,7 +9806,7 @@
         <v>111</v>
       </c>
       <c r="Y110" s="3">
-        <f>N53</f>
+        <f t="shared" si="9"/>
         <v>51</v>
       </c>
       <c r="Z110" s="1">
@@ -9700,7 +9817,7 @@
         <v>108</v>
       </c>
       <c r="AF110" s="3">
-        <f>N55</f>
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
       <c r="AG110" s="1">
@@ -9711,8 +9828,11 @@
         <v>108</v>
       </c>
       <c r="AI110" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>108</v>
+      </c>
+      <c r="AJ110" s="1" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="111" spans="14:36" x14ac:dyDescent="0.3">
@@ -9736,7 +9856,7 @@
         <v>112</v>
       </c>
       <c r="Y111" s="3">
-        <f>N54</f>
+        <f t="shared" si="9"/>
         <v>52</v>
       </c>
       <c r="Z111" s="1">
@@ -9747,7 +9867,7 @@
         <v>109</v>
       </c>
       <c r="AF111" s="3">
-        <f>N56</f>
+        <f t="shared" ref="AF111:AF142" si="11">N56</f>
         <v>54</v>
       </c>
       <c r="AG111" s="1">
@@ -9758,7 +9878,7 @@
         <v>109</v>
       </c>
       <c r="AI111" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>109</v>
       </c>
       <c r="AJ111" s="1" t="s">
@@ -9783,7 +9903,7 @@
         <v>113</v>
       </c>
       <c r="Y112" s="3">
-        <f>N55</f>
+        <f t="shared" si="9"/>
         <v>53</v>
       </c>
       <c r="Z112" s="1">
@@ -9794,7 +9914,7 @@
         <v>110</v>
       </c>
       <c r="AF112" s="3">
-        <f>N57</f>
+        <f t="shared" si="11"/>
         <v>55</v>
       </c>
       <c r="AG112" s="1">
@@ -9805,7 +9925,7 @@
         <v>110</v>
       </c>
       <c r="AI112" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
       <c r="AJ112" s="1" t="s">
@@ -9830,7 +9950,7 @@
         <v>114</v>
       </c>
       <c r="Y113" s="3">
-        <f>N56</f>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="Z113" s="1">
@@ -9841,7 +9961,7 @@
         <v>111</v>
       </c>
       <c r="AF113" s="3">
-        <f>N58</f>
+        <f t="shared" si="11"/>
         <v>56</v>
       </c>
       <c r="AG113" s="1">
@@ -9852,7 +9972,7 @@
         <v>111</v>
       </c>
       <c r="AI113" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>111</v>
       </c>
       <c r="AJ113" s="1" t="s">
@@ -9877,7 +9997,7 @@
         <v>115</v>
       </c>
       <c r="Y114" s="3">
-        <f>N57</f>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="Z114" s="1">
@@ -9888,7 +10008,7 @@
         <v>112</v>
       </c>
       <c r="AF114" s="3">
-        <f>N59</f>
+        <f t="shared" si="11"/>
         <v>57</v>
       </c>
       <c r="AG114" s="1">
@@ -9899,7 +10019,7 @@
         <v>112</v>
       </c>
       <c r="AI114" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>112</v>
       </c>
       <c r="AJ114" s="3" t="s">
@@ -9924,7 +10044,7 @@
         <v>116</v>
       </c>
       <c r="Y115" s="3">
-        <f>N58</f>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="Z115" s="1">
@@ -9935,7 +10055,7 @@
         <v>113</v>
       </c>
       <c r="AF115" s="3">
-        <f>N60</f>
+        <f t="shared" si="11"/>
         <v>58</v>
       </c>
       <c r="AG115" s="1">
@@ -9946,7 +10066,7 @@
         <v>113</v>
       </c>
       <c r="AI115" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>113</v>
       </c>
       <c r="AJ115" s="1" t="s">
@@ -9974,7 +10094,7 @@
         <v>117</v>
       </c>
       <c r="Y116" s="3">
-        <f>N59</f>
+        <f t="shared" si="9"/>
         <v>57</v>
       </c>
       <c r="Z116" s="1">
@@ -9985,7 +10105,7 @@
         <v>114</v>
       </c>
       <c r="AF116" s="3">
-        <f>N61</f>
+        <f t="shared" si="11"/>
         <v>59</v>
       </c>
       <c r="AG116" s="1">
@@ -9996,7 +10116,7 @@
         <v>114</v>
       </c>
       <c r="AI116" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>114</v>
       </c>
       <c r="AJ116" s="1" t="s">
@@ -10024,7 +10144,7 @@
         <v>118</v>
       </c>
       <c r="Y117" s="3">
-        <f>N60</f>
+        <f t="shared" si="9"/>
         <v>58</v>
       </c>
       <c r="Z117" s="1">
@@ -10035,7 +10155,7 @@
         <v>115</v>
       </c>
       <c r="AF117" s="3">
-        <f>N62</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AG117" s="1">
@@ -10046,7 +10166,7 @@
         <v>115</v>
       </c>
       <c r="AI117" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>115</v>
       </c>
       <c r="AJ117" s="1" t="s">
@@ -10074,7 +10194,7 @@
         <v>119</v>
       </c>
       <c r="Y118" s="3">
-        <f>N61</f>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="Z118" s="1">
@@ -10085,7 +10205,7 @@
         <v>116</v>
       </c>
       <c r="AF118" s="3">
-        <f>N63</f>
+        <f t="shared" si="11"/>
         <v>61</v>
       </c>
       <c r="AG118" s="1">
@@ -10096,7 +10216,7 @@
         <v>116</v>
       </c>
       <c r="AI118" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>116</v>
       </c>
       <c r="AJ118" s="1" t="s">
@@ -10121,7 +10241,7 @@
         <v>120</v>
       </c>
       <c r="Y119" s="3">
-        <f>N62</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Z119" s="1">
@@ -10132,7 +10252,7 @@
         <v>117</v>
       </c>
       <c r="AF119" s="3">
-        <f>N64</f>
+        <f t="shared" si="11"/>
         <v>62</v>
       </c>
       <c r="AG119" s="1">
@@ -10143,7 +10263,7 @@
         <v>117</v>
       </c>
       <c r="AI119" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>117</v>
       </c>
       <c r="AJ119" s="1" t="s">
@@ -10168,7 +10288,7 @@
         <v>121</v>
       </c>
       <c r="Y120" s="3">
-        <f>N63</f>
+        <f t="shared" si="9"/>
         <v>61</v>
       </c>
       <c r="Z120" s="1">
@@ -10179,7 +10299,7 @@
         <v>118</v>
       </c>
       <c r="AF120" s="3">
-        <f>N65</f>
+        <f t="shared" si="11"/>
         <v>63</v>
       </c>
       <c r="AG120" s="1">
@@ -10190,7 +10310,7 @@
         <v>118</v>
       </c>
       <c r="AI120" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>118</v>
       </c>
       <c r="AJ120" s="1" t="s">
@@ -10215,7 +10335,7 @@
         <v>122</v>
       </c>
       <c r="Y121" s="3">
-        <f>N64</f>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="Z121" s="1">
@@ -10226,7 +10346,7 @@
         <v>119</v>
       </c>
       <c r="AF121" s="3">
-        <f>N66</f>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="AG121" s="1">
@@ -10237,7 +10357,7 @@
         <v>119</v>
       </c>
       <c r="AI121" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>119</v>
       </c>
       <c r="AJ121" s="1" t="s">
@@ -10262,7 +10382,7 @@
         <v>123</v>
       </c>
       <c r="Y122" s="3">
-        <f>N65</f>
+        <f t="shared" si="9"/>
         <v>63</v>
       </c>
       <c r="Z122" s="1">
@@ -10273,7 +10393,7 @@
         <v>120</v>
       </c>
       <c r="AF122" s="3">
-        <f>N67</f>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="AG122" s="1">
@@ -10284,7 +10404,7 @@
         <v>120</v>
       </c>
       <c r="AI122" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
       <c r="AJ122" s="1" t="s">
@@ -10309,7 +10429,7 @@
         <v>124</v>
       </c>
       <c r="Y123" s="3">
-        <f>N66</f>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="Z123" s="1">
@@ -10320,7 +10440,7 @@
         <v>121</v>
       </c>
       <c r="AF123" s="3">
-        <f>N68</f>
+        <f t="shared" si="11"/>
         <v>66</v>
       </c>
       <c r="AG123" s="1">
@@ -10331,7 +10451,7 @@
         <v>121</v>
       </c>
       <c r="AI123" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>121</v>
       </c>
       <c r="AJ123" s="1" t="s">
@@ -10356,7 +10476,7 @@
         <v>125</v>
       </c>
       <c r="Y124" s="3">
-        <f>N67</f>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="Z124" s="1">
@@ -10367,7 +10487,7 @@
         <v>122</v>
       </c>
       <c r="AF124" s="3">
-        <f>N69</f>
+        <f t="shared" si="11"/>
         <v>67</v>
       </c>
       <c r="AG124" s="1">
@@ -10378,7 +10498,7 @@
         <v>122</v>
       </c>
       <c r="AI124" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>122</v>
       </c>
       <c r="AJ124" s="1" t="s">
@@ -10403,7 +10523,7 @@
         <v>126</v>
       </c>
       <c r="Y125" s="3">
-        <f>N68</f>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="Z125" s="1">
@@ -10414,7 +10534,7 @@
         <v>123</v>
       </c>
       <c r="AF125" s="3">
-        <f>N70</f>
+        <f t="shared" si="11"/>
         <v>68</v>
       </c>
       <c r="AG125" s="1">
@@ -10425,7 +10545,7 @@
         <v>123</v>
       </c>
       <c r="AI125" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>123</v>
       </c>
       <c r="AJ125" s="1" t="s">
@@ -10450,7 +10570,7 @@
         <v>127</v>
       </c>
       <c r="Y126" s="3">
-        <f>N69</f>
+        <f t="shared" si="9"/>
         <v>67</v>
       </c>
       <c r="Z126" s="1">
@@ -10461,7 +10581,7 @@
         <v>124</v>
       </c>
       <c r="AF126" s="3">
-        <f>N71</f>
+        <f t="shared" si="11"/>
         <v>69</v>
       </c>
       <c r="AG126" s="1">
@@ -10472,7 +10592,7 @@
         <v>124</v>
       </c>
       <c r="AI126" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>124</v>
       </c>
       <c r="AJ126" s="1" t="s">
@@ -10497,7 +10617,7 @@
         <v>128</v>
       </c>
       <c r="Y127" s="3">
-        <f>N70</f>
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
       <c r="Z127" s="1">
@@ -10508,7 +10628,7 @@
         <v>125</v>
       </c>
       <c r="AF127" s="3">
-        <f>N72</f>
+        <f t="shared" si="11"/>
         <v>70</v>
       </c>
       <c r="AG127" s="1">
@@ -10519,7 +10639,7 @@
         <v>125</v>
       </c>
       <c r="AI127" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="AJ127" s="1" t="s">
@@ -10544,7 +10664,7 @@
         <v>129</v>
       </c>
       <c r="Y128" s="3">
-        <f>N71</f>
+        <f t="shared" si="9"/>
         <v>69</v>
       </c>
       <c r="Z128" s="1">
@@ -10555,7 +10675,7 @@
         <v>126</v>
       </c>
       <c r="AF128" s="3">
-        <f>N73</f>
+        <f t="shared" si="11"/>
         <v>71</v>
       </c>
       <c r="AG128" s="1">
@@ -10566,7 +10686,7 @@
         <v>126</v>
       </c>
       <c r="AI128" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>126</v>
       </c>
       <c r="AJ128" s="1" t="s">
@@ -10591,7 +10711,7 @@
         <v>130</v>
       </c>
       <c r="Y129" s="3">
-        <f>N72</f>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="Z129" s="1">
@@ -10602,7 +10722,7 @@
         <v>127</v>
       </c>
       <c r="AF129" s="3">
-        <f>N74</f>
+        <f t="shared" si="11"/>
         <v>72</v>
       </c>
       <c r="AG129" s="1">
@@ -10613,7 +10733,7 @@
         <v>127</v>
       </c>
       <c r="AI129" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>127</v>
       </c>
       <c r="AJ129" s="1" t="s">
@@ -10638,7 +10758,7 @@
         <v>131</v>
       </c>
       <c r="Y130" s="3">
-        <f>N73</f>
+        <f t="shared" si="9"/>
         <v>71</v>
       </c>
       <c r="Z130" s="1">
@@ -10649,7 +10769,7 @@
         <v>128</v>
       </c>
       <c r="AF130" s="3">
-        <f>N75</f>
+        <f t="shared" si="11"/>
         <v>73</v>
       </c>
       <c r="AG130" s="1">
@@ -10660,7 +10780,7 @@
         <v>128</v>
       </c>
       <c r="AI130" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="AJ130" s="1" t="s">
@@ -10685,7 +10805,7 @@
         <v>132</v>
       </c>
       <c r="Y131" s="3">
-        <f>N74</f>
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="Z131" s="1">
@@ -10696,7 +10816,7 @@
         <v>129</v>
       </c>
       <c r="AF131" s="3">
-        <f>N76</f>
+        <f t="shared" si="11"/>
         <v>74</v>
       </c>
       <c r="AG131" s="1">
@@ -10707,7 +10827,7 @@
         <v>129</v>
       </c>
       <c r="AI131" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>129</v>
       </c>
       <c r="AJ131" s="1" t="s">
@@ -10732,7 +10852,7 @@
         <v>133</v>
       </c>
       <c r="Y132" s="3">
-        <f>N75</f>
+        <f t="shared" ref="Y132:Y163" si="12">N75</f>
         <v>73</v>
       </c>
       <c r="Z132" s="1">
@@ -10743,7 +10863,7 @@
         <v>130</v>
       </c>
       <c r="AF132" s="3">
-        <f>N77</f>
+        <f t="shared" si="11"/>
         <v>75</v>
       </c>
       <c r="AG132" s="1">
@@ -10754,7 +10874,7 @@
         <v>130</v>
       </c>
       <c r="AI132" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>130</v>
       </c>
       <c r="AJ132" s="1" t="s">
@@ -10779,7 +10899,7 @@
         <v>134</v>
       </c>
       <c r="Y133" s="3">
-        <f>N76</f>
+        <f t="shared" si="12"/>
         <v>74</v>
       </c>
       <c r="Z133" s="1">
@@ -10790,7 +10910,7 @@
         <v>131</v>
       </c>
       <c r="AF133" s="3">
-        <f>N78</f>
+        <f t="shared" si="11"/>
         <v>76</v>
       </c>
       <c r="AG133" s="1">
@@ -10801,7 +10921,7 @@
         <v>131</v>
       </c>
       <c r="AI133" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>131</v>
       </c>
       <c r="AJ133" s="1" t="s">
@@ -10826,7 +10946,7 @@
         <v>135</v>
       </c>
       <c r="Y134" s="3">
-        <f>N77</f>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
       <c r="Z134" s="1">
@@ -10837,7 +10957,7 @@
         <v>132</v>
       </c>
       <c r="AF134" s="3">
-        <f>N79</f>
+        <f t="shared" si="11"/>
         <v>77</v>
       </c>
       <c r="AG134" s="1">
@@ -10848,7 +10968,7 @@
         <v>132</v>
       </c>
       <c r="AI134" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>132</v>
       </c>
       <c r="AJ134" s="1" t="s">
@@ -10873,7 +10993,7 @@
         <v>136</v>
       </c>
       <c r="Y135" s="3">
-        <f>N78</f>
+        <f t="shared" si="12"/>
         <v>76</v>
       </c>
       <c r="Z135" s="1">
@@ -10884,7 +11004,7 @@
         <v>133</v>
       </c>
       <c r="AF135" s="3">
-        <f>N80</f>
+        <f t="shared" si="11"/>
         <v>78</v>
       </c>
       <c r="AG135" s="1">
@@ -10895,7 +11015,7 @@
         <v>133</v>
       </c>
       <c r="AI135" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>133</v>
       </c>
       <c r="AJ135" s="1" t="s">
@@ -10920,7 +11040,7 @@
         <v>137</v>
       </c>
       <c r="Y136" s="3">
-        <f>N79</f>
+        <f t="shared" si="12"/>
         <v>77</v>
       </c>
       <c r="Z136" s="1">
@@ -10931,7 +11051,7 @@
         <v>134</v>
       </c>
       <c r="AF136" s="3">
-        <f>N81</f>
+        <f t="shared" si="11"/>
         <v>79</v>
       </c>
       <c r="AG136" s="1">
@@ -10942,7 +11062,7 @@
         <v>134</v>
       </c>
       <c r="AI136" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>134</v>
       </c>
       <c r="AJ136" s="1" t="s">
@@ -10967,7 +11087,7 @@
         <v>138</v>
       </c>
       <c r="Y137" s="3">
-        <f>N80</f>
+        <f t="shared" si="12"/>
         <v>78</v>
       </c>
       <c r="Z137" s="1">
@@ -10978,7 +11098,7 @@
         <v>135</v>
       </c>
       <c r="AF137" s="3">
-        <f>N82</f>
+        <f t="shared" si="11"/>
         <v>80</v>
       </c>
       <c r="AG137" s="1">
@@ -10989,7 +11109,7 @@
         <v>135</v>
       </c>
       <c r="AI137" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
       <c r="AJ137" s="1" t="s">
@@ -11014,7 +11134,7 @@
         <v>139</v>
       </c>
       <c r="Y138" s="3">
-        <f>N81</f>
+        <f t="shared" si="12"/>
         <v>79</v>
       </c>
       <c r="Z138" s="1">
@@ -11025,7 +11145,7 @@
         <v>136</v>
       </c>
       <c r="AF138" s="3">
-        <f>N83</f>
+        <f t="shared" si="11"/>
         <v>81</v>
       </c>
       <c r="AG138" s="1">
@@ -11036,7 +11156,7 @@
         <v>136</v>
       </c>
       <c r="AI138" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>136</v>
       </c>
       <c r="AJ138" s="1" t="s">
@@ -11061,7 +11181,7 @@
         <v>140</v>
       </c>
       <c r="Y139" s="3">
-        <f>N82</f>
+        <f t="shared" si="12"/>
         <v>80</v>
       </c>
       <c r="Z139" s="1">
@@ -11072,7 +11192,7 @@
         <v>137</v>
       </c>
       <c r="AF139" s="3">
-        <f>N84</f>
+        <f t="shared" si="11"/>
         <v>82</v>
       </c>
       <c r="AG139" s="1">
@@ -11083,7 +11203,7 @@
         <v>137</v>
       </c>
       <c r="AI139" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>137</v>
       </c>
       <c r="AJ139" s="1" t="s">
@@ -11108,7 +11228,7 @@
         <v>141</v>
       </c>
       <c r="Y140" s="3">
-        <f>N83</f>
+        <f t="shared" si="12"/>
         <v>81</v>
       </c>
       <c r="Z140" s="1">
@@ -11119,7 +11239,7 @@
         <v>138</v>
       </c>
       <c r="AF140" s="3">
-        <f>N85</f>
+        <f t="shared" si="11"/>
         <v>83</v>
       </c>
       <c r="AG140" s="1">
@@ -11130,7 +11250,7 @@
         <v>138</v>
       </c>
       <c r="AI140" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>138</v>
       </c>
       <c r="AJ140" s="1" t="s">
@@ -11142,7 +11262,7 @@
         <v>142</v>
       </c>
       <c r="Y141" s="3">
-        <f>N84</f>
+        <f t="shared" si="12"/>
         <v>82</v>
       </c>
       <c r="Z141" s="1">
@@ -11153,7 +11273,7 @@
         <v>139</v>
       </c>
       <c r="AF141" s="3">
-        <f>N86</f>
+        <f t="shared" si="11"/>
         <v>84</v>
       </c>
       <c r="AG141" s="1">
@@ -11166,7 +11286,7 @@
         <v>143</v>
       </c>
       <c r="Y142" s="3">
-        <f>N85</f>
+        <f t="shared" si="12"/>
         <v>83</v>
       </c>
       <c r="Z142" s="1">
@@ -11177,7 +11297,7 @@
         <v>140</v>
       </c>
       <c r="AF142" s="3">
-        <f>N87</f>
+        <f t="shared" si="11"/>
         <v>85</v>
       </c>
       <c r="AG142" s="1">
@@ -11190,7 +11310,7 @@
         <v>144</v>
       </c>
       <c r="Y143" s="3">
-        <f>N86</f>
+        <f t="shared" si="12"/>
         <v>84</v>
       </c>
       <c r="Z143" s="1">
@@ -11201,7 +11321,7 @@
         <v>141</v>
       </c>
       <c r="AF143" s="3">
-        <f>N88</f>
+        <f t="shared" ref="AF143:AF174" si="13">N88</f>
         <v>86</v>
       </c>
       <c r="AG143" s="1">
@@ -11214,7 +11334,7 @@
         <v>145</v>
       </c>
       <c r="Y144" s="3">
-        <f>N87</f>
+        <f t="shared" si="12"/>
         <v>85</v>
       </c>
       <c r="Z144" s="1">
@@ -11225,7 +11345,7 @@
         <v>142</v>
       </c>
       <c r="AF144" s="3">
-        <f>N89</f>
+        <f t="shared" si="13"/>
         <v>87</v>
       </c>
       <c r="AG144" s="1">
@@ -11238,7 +11358,7 @@
         <v>146</v>
       </c>
       <c r="Y145" s="3">
-        <f>N88</f>
+        <f t="shared" si="12"/>
         <v>86</v>
       </c>
       <c r="Z145" s="1">
@@ -11249,7 +11369,7 @@
         <v>143</v>
       </c>
       <c r="AF145" s="3">
-        <f>N90</f>
+        <f t="shared" si="13"/>
         <v>88</v>
       </c>
       <c r="AG145" s="1">
@@ -11262,7 +11382,7 @@
         <v>147</v>
       </c>
       <c r="Y146" s="3">
-        <f>N89</f>
+        <f t="shared" si="12"/>
         <v>87</v>
       </c>
       <c r="Z146" s="1">
@@ -11273,7 +11393,7 @@
         <v>144</v>
       </c>
       <c r="AF146" s="3">
-        <f>N91</f>
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="AG146" s="1">
@@ -11286,7 +11406,7 @@
         <v>148</v>
       </c>
       <c r="Y147" s="3">
-        <f>N90</f>
+        <f t="shared" si="12"/>
         <v>88</v>
       </c>
       <c r="Z147" s="1">
@@ -11297,7 +11417,7 @@
         <v>145</v>
       </c>
       <c r="AF147" s="3">
-        <f>N92</f>
+        <f t="shared" si="13"/>
         <v>90</v>
       </c>
       <c r="AG147" s="1">
@@ -11310,7 +11430,7 @@
         <v>149</v>
       </c>
       <c r="Y148" s="3">
-        <f>N91</f>
+        <f t="shared" si="12"/>
         <v>89</v>
       </c>
       <c r="Z148" s="1">
@@ -11321,7 +11441,7 @@
         <v>146</v>
       </c>
       <c r="AF148" s="3">
-        <f>N93</f>
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="AG148" s="1">
@@ -11334,7 +11454,7 @@
         <v>150</v>
       </c>
       <c r="Y149" s="3">
-        <f>N92</f>
+        <f t="shared" si="12"/>
         <v>90</v>
       </c>
       <c r="Z149" s="1">
@@ -11345,7 +11465,7 @@
         <v>147</v>
       </c>
       <c r="AF149" s="3">
-        <f>N94</f>
+        <f t="shared" si="13"/>
         <v>92</v>
       </c>
       <c r="AG149" s="1">
@@ -11358,7 +11478,7 @@
         <v>151</v>
       </c>
       <c r="Y150" s="3">
-        <f>N93</f>
+        <f t="shared" si="12"/>
         <v>91</v>
       </c>
       <c r="Z150" s="1">
@@ -11369,7 +11489,7 @@
         <v>148</v>
       </c>
       <c r="AF150" s="3">
-        <f>N95</f>
+        <f t="shared" si="13"/>
         <v>93</v>
       </c>
       <c r="AG150" s="1">
@@ -11382,7 +11502,7 @@
         <v>152</v>
       </c>
       <c r="Y151" s="3">
-        <f>N94</f>
+        <f t="shared" si="12"/>
         <v>92</v>
       </c>
       <c r="Z151" s="1">
@@ -11393,7 +11513,7 @@
         <v>149</v>
       </c>
       <c r="AF151" s="3">
-        <f>N96</f>
+        <f t="shared" si="13"/>
         <v>94</v>
       </c>
       <c r="AG151" s="1">
@@ -11406,7 +11526,7 @@
         <v>153</v>
       </c>
       <c r="Y152" s="3">
-        <f>N95</f>
+        <f t="shared" si="12"/>
         <v>93</v>
       </c>
       <c r="Z152" s="1">
@@ -11417,7 +11537,7 @@
         <v>150</v>
       </c>
       <c r="AF152" s="3">
-        <f>N97</f>
+        <f t="shared" si="13"/>
         <v>95</v>
       </c>
       <c r="AG152" s="1">
@@ -11430,7 +11550,7 @@
         <v>154</v>
       </c>
       <c r="Y153" s="3">
-        <f>N96</f>
+        <f t="shared" si="12"/>
         <v>94</v>
       </c>
       <c r="Z153" s="1">
@@ -11441,7 +11561,7 @@
         <v>151</v>
       </c>
       <c r="AF153" s="3">
-        <f>N98</f>
+        <f t="shared" si="13"/>
         <v>96</v>
       </c>
       <c r="AG153" s="1">
@@ -11454,7 +11574,7 @@
         <v>155</v>
       </c>
       <c r="Y154" s="3">
-        <f>N97</f>
+        <f t="shared" si="12"/>
         <v>95</v>
       </c>
       <c r="Z154" s="1">
@@ -11465,7 +11585,7 @@
         <v>152</v>
       </c>
       <c r="AF154" s="3">
-        <f>N99</f>
+        <f t="shared" si="13"/>
         <v>97</v>
       </c>
       <c r="AG154" s="1">
@@ -11478,7 +11598,7 @@
         <v>156</v>
       </c>
       <c r="Y155" s="3">
-        <f>N76</f>
+        <f t="shared" ref="Y155:Y189" si="14">N76</f>
         <v>74</v>
       </c>
       <c r="Z155" s="1">
@@ -11489,7 +11609,7 @@
         <v>153</v>
       </c>
       <c r="AF155" s="3">
-        <f>N100</f>
+        <f t="shared" si="13"/>
         <v>98</v>
       </c>
       <c r="AG155" s="1">
@@ -11502,7 +11622,7 @@
         <v>157</v>
       </c>
       <c r="Y156" s="3">
-        <f>N77</f>
+        <f t="shared" si="14"/>
         <v>75</v>
       </c>
       <c r="Z156" s="1">
@@ -11513,7 +11633,7 @@
         <v>154</v>
       </c>
       <c r="AF156" s="3">
-        <f>N101</f>
+        <f t="shared" si="13"/>
         <v>99</v>
       </c>
       <c r="AG156" s="1">
@@ -11526,7 +11646,7 @@
         <v>158</v>
       </c>
       <c r="Y157" s="3">
-        <f>N78</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="Z157" s="1">
@@ -11537,7 +11657,7 @@
         <v>155</v>
       </c>
       <c r="AF157" s="3">
-        <f>N102</f>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="AG157" s="1">
@@ -11550,7 +11670,7 @@
         <v>159</v>
       </c>
       <c r="Y158" s="3">
-        <f>N79</f>
+        <f t="shared" si="14"/>
         <v>77</v>
       </c>
       <c r="Z158" s="1">
@@ -11561,7 +11681,7 @@
         <v>156</v>
       </c>
       <c r="AF158" s="3">
-        <f>N103</f>
+        <f t="shared" si="13"/>
         <v>101</v>
       </c>
       <c r="AG158" s="1">
@@ -11574,7 +11694,7 @@
         <v>160</v>
       </c>
       <c r="Y159" s="3">
-        <f>N80</f>
+        <f t="shared" si="14"/>
         <v>78</v>
       </c>
       <c r="Z159" s="1">
@@ -11585,7 +11705,7 @@
         <v>157</v>
       </c>
       <c r="AF159" s="3">
-        <f>N104</f>
+        <f t="shared" si="13"/>
         <v>102</v>
       </c>
       <c r="AG159" s="1">
@@ -11598,7 +11718,7 @@
         <v>161</v>
       </c>
       <c r="Y160" s="3">
-        <f>N81</f>
+        <f t="shared" si="14"/>
         <v>79</v>
       </c>
       <c r="Z160" s="1">
@@ -11609,7 +11729,7 @@
         <v>158</v>
       </c>
       <c r="AF160" s="3">
-        <f>N105</f>
+        <f t="shared" si="13"/>
         <v>103</v>
       </c>
       <c r="AG160" s="1">
@@ -11622,7 +11742,7 @@
         <v>162</v>
       </c>
       <c r="Y161" s="3">
-        <f>N82</f>
+        <f t="shared" si="14"/>
         <v>80</v>
       </c>
       <c r="Z161" s="1">
@@ -11633,7 +11753,7 @@
         <v>159</v>
       </c>
       <c r="AF161" s="3">
-        <f>N106</f>
+        <f t="shared" si="13"/>
         <v>104</v>
       </c>
       <c r="AG161" s="1">
@@ -11646,7 +11766,7 @@
         <v>163</v>
       </c>
       <c r="Y162" s="3">
-        <f>N83</f>
+        <f t="shared" si="14"/>
         <v>81</v>
       </c>
       <c r="Z162" s="1">
@@ -11657,7 +11777,7 @@
         <v>160</v>
       </c>
       <c r="AF162" s="3">
-        <f>N107</f>
+        <f t="shared" si="13"/>
         <v>105</v>
       </c>
       <c r="AG162" s="1">
@@ -11670,7 +11790,7 @@
         <v>164</v>
       </c>
       <c r="Y163" s="3">
-        <f>N84</f>
+        <f t="shared" si="14"/>
         <v>82</v>
       </c>
       <c r="Z163" s="1">
@@ -11681,7 +11801,7 @@
         <v>161</v>
       </c>
       <c r="AF163" s="3">
-        <f>N108</f>
+        <f t="shared" si="13"/>
         <v>106</v>
       </c>
       <c r="AG163" s="1">
@@ -11694,7 +11814,7 @@
         <v>165</v>
       </c>
       <c r="Y164" s="3">
-        <f>N85</f>
+        <f t="shared" si="14"/>
         <v>83</v>
       </c>
       <c r="Z164" s="1">
@@ -11705,7 +11825,7 @@
         <v>162</v>
       </c>
       <c r="AF164" s="3">
-        <f>N109</f>
+        <f t="shared" si="13"/>
         <v>107</v>
       </c>
       <c r="AG164" s="1">
@@ -11718,7 +11838,7 @@
         <v>166</v>
       </c>
       <c r="Y165" s="3">
-        <f>N86</f>
+        <f t="shared" si="14"/>
         <v>84</v>
       </c>
       <c r="Z165" s="1">
@@ -11729,7 +11849,7 @@
         <v>163</v>
       </c>
       <c r="AF165" s="3">
-        <f>N110</f>
+        <f t="shared" si="13"/>
         <v>108</v>
       </c>
       <c r="AG165" s="1">
@@ -11742,7 +11862,7 @@
         <v>167</v>
       </c>
       <c r="Y166" s="3">
-        <f>N87</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="Z166" s="1">
@@ -11753,7 +11873,7 @@
         <v>164</v>
       </c>
       <c r="AF166" s="3">
-        <f>N111</f>
+        <f t="shared" si="13"/>
         <v>109</v>
       </c>
       <c r="AG166" s="1">
@@ -11766,7 +11886,7 @@
         <v>168</v>
       </c>
       <c r="Y167" s="3">
-        <f>N88</f>
+        <f t="shared" si="14"/>
         <v>86</v>
       </c>
       <c r="Z167" s="1">
@@ -11777,7 +11897,7 @@
         <v>165</v>
       </c>
       <c r="AF167" s="3">
-        <f>N112</f>
+        <f t="shared" si="13"/>
         <v>110</v>
       </c>
       <c r="AG167" s="1">
@@ -11790,7 +11910,7 @@
         <v>169</v>
       </c>
       <c r="Y168" s="3">
-        <f>N89</f>
+        <f t="shared" si="14"/>
         <v>87</v>
       </c>
       <c r="Z168" s="1">
@@ -11801,7 +11921,7 @@
         <v>166</v>
       </c>
       <c r="AF168" s="3">
-        <f>N113</f>
+        <f t="shared" si="13"/>
         <v>111</v>
       </c>
       <c r="AG168" s="1">
@@ -11814,7 +11934,7 @@
         <v>170</v>
       </c>
       <c r="Y169" s="3">
-        <f>N90</f>
+        <f t="shared" si="14"/>
         <v>88</v>
       </c>
       <c r="Z169" s="1">
@@ -11825,7 +11945,7 @@
         <v>167</v>
       </c>
       <c r="AF169" s="3">
-        <f>N114</f>
+        <f t="shared" si="13"/>
         <v>112</v>
       </c>
       <c r="AG169" s="1">
@@ -11838,7 +11958,7 @@
         <v>171</v>
       </c>
       <c r="Y170" s="3">
-        <f>N91</f>
+        <f t="shared" si="14"/>
         <v>89</v>
       </c>
       <c r="Z170" s="1">
@@ -11849,7 +11969,7 @@
         <v>168</v>
       </c>
       <c r="AF170" s="3">
-        <f>N115</f>
+        <f t="shared" si="13"/>
         <v>113</v>
       </c>
       <c r="AG170" s="1">
@@ -11862,7 +11982,7 @@
         <v>172</v>
       </c>
       <c r="Y171" s="3">
-        <f>N92</f>
+        <f t="shared" si="14"/>
         <v>90</v>
       </c>
       <c r="Z171" s="1">
@@ -11873,7 +11993,7 @@
         <v>169</v>
       </c>
       <c r="AF171" s="3">
-        <f>N116</f>
+        <f t="shared" si="13"/>
         <v>114</v>
       </c>
       <c r="AG171" s="1">
@@ -11886,7 +12006,7 @@
         <v>173</v>
       </c>
       <c r="Y172" s="3">
-        <f>N93</f>
+        <f t="shared" si="14"/>
         <v>91</v>
       </c>
       <c r="Z172" s="1">
@@ -11897,7 +12017,7 @@
         <v>170</v>
       </c>
       <c r="AF172" s="3">
-        <f>N117</f>
+        <f t="shared" si="13"/>
         <v>115</v>
       </c>
       <c r="AG172" s="1">
@@ -11910,7 +12030,7 @@
         <v>174</v>
       </c>
       <c r="Y173" s="3">
-        <f>N94</f>
+        <f t="shared" si="14"/>
         <v>92</v>
       </c>
       <c r="Z173" s="1">
@@ -11921,7 +12041,7 @@
         <v>171</v>
       </c>
       <c r="AF173" s="3">
-        <f>N118</f>
+        <f t="shared" si="13"/>
         <v>116</v>
       </c>
       <c r="AG173" s="1">
@@ -11934,7 +12054,7 @@
         <v>175</v>
       </c>
       <c r="Y174" s="3">
-        <f>N95</f>
+        <f t="shared" si="14"/>
         <v>93</v>
       </c>
       <c r="Z174" s="1">
@@ -11945,7 +12065,7 @@
         <v>172</v>
       </c>
       <c r="AF174" s="3">
-        <f>N119</f>
+        <f t="shared" si="13"/>
         <v>117</v>
       </c>
       <c r="AG174" s="1">
@@ -11958,7 +12078,7 @@
         <v>176</v>
       </c>
       <c r="Y175" s="3">
-        <f>N96</f>
+        <f t="shared" si="14"/>
         <v>94</v>
       </c>
       <c r="Z175" s="1">
@@ -11969,7 +12089,7 @@
         <v>173</v>
       </c>
       <c r="AF175" s="3">
-        <f>N114</f>
+        <f t="shared" ref="AF175:AF201" si="15">N114</f>
         <v>112</v>
       </c>
       <c r="AG175" s="1">
@@ -11982,7 +12102,7 @@
         <v>177</v>
       </c>
       <c r="Y176" s="3">
-        <f>N97</f>
+        <f t="shared" si="14"/>
         <v>95</v>
       </c>
       <c r="Z176" s="1">
@@ -11993,7 +12113,7 @@
         <v>174</v>
       </c>
       <c r="AF176" s="3">
-        <f>N115</f>
+        <f t="shared" si="15"/>
         <v>113</v>
       </c>
       <c r="AG176" s="1">
@@ -12006,7 +12126,7 @@
         <v>178</v>
       </c>
       <c r="Y177" s="3">
-        <f>N98</f>
+        <f t="shared" si="14"/>
         <v>96</v>
       </c>
       <c r="Z177" s="1">
@@ -12017,7 +12137,7 @@
         <v>175</v>
       </c>
       <c r="AF177" s="3">
-        <f>N116</f>
+        <f t="shared" si="15"/>
         <v>114</v>
       </c>
       <c r="AG177" s="1">
@@ -12030,7 +12150,7 @@
         <v>179</v>
       </c>
       <c r="Y178" s="3">
-        <f>N99</f>
+        <f t="shared" si="14"/>
         <v>97</v>
       </c>
       <c r="Z178" s="1">
@@ -12041,7 +12161,7 @@
         <v>176</v>
       </c>
       <c r="AF178" s="3">
-        <f>N117</f>
+        <f t="shared" si="15"/>
         <v>115</v>
       </c>
       <c r="AG178" s="1">
@@ -12054,7 +12174,7 @@
         <v>180</v>
       </c>
       <c r="Y179" s="3">
-        <f>N100</f>
+        <f t="shared" si="14"/>
         <v>98</v>
       </c>
       <c r="Z179" s="1">
@@ -12065,7 +12185,7 @@
         <v>177</v>
       </c>
       <c r="AF179" s="3">
-        <f>N118</f>
+        <f t="shared" si="15"/>
         <v>116</v>
       </c>
       <c r="AG179" s="1">
@@ -12078,7 +12198,7 @@
         <v>181</v>
       </c>
       <c r="Y180" s="3">
-        <f>N101</f>
+        <f t="shared" si="14"/>
         <v>99</v>
       </c>
       <c r="Z180" s="1">
@@ -12089,7 +12209,7 @@
         <v>178</v>
       </c>
       <c r="AF180" s="3">
-        <f>N119</f>
+        <f t="shared" si="15"/>
         <v>117</v>
       </c>
       <c r="AG180" s="1">
@@ -12102,7 +12222,7 @@
         <v>182</v>
       </c>
       <c r="Y181" s="3">
-        <f>N102</f>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="Z181" s="1">
@@ -12113,7 +12233,7 @@
         <v>179</v>
       </c>
       <c r="AF181" s="3">
-        <f>N120</f>
+        <f t="shared" si="15"/>
         <v>118</v>
       </c>
       <c r="AG181" s="1">
@@ -12126,7 +12246,7 @@
         <v>183</v>
       </c>
       <c r="Y182" s="3">
-        <f>N103</f>
+        <f t="shared" si="14"/>
         <v>101</v>
       </c>
       <c r="Z182" s="1">
@@ -12137,7 +12257,7 @@
         <v>180</v>
       </c>
       <c r="AF182" s="3">
-        <f>N121</f>
+        <f t="shared" si="15"/>
         <v>119</v>
       </c>
       <c r="AG182" s="1">
@@ -12150,7 +12270,7 @@
         <v>184</v>
       </c>
       <c r="Y183" s="3">
-        <f>N104</f>
+        <f t="shared" si="14"/>
         <v>102</v>
       </c>
       <c r="Z183" s="1">
@@ -12161,7 +12281,7 @@
         <v>181</v>
       </c>
       <c r="AF183" s="3">
-        <f>N122</f>
+        <f t="shared" si="15"/>
         <v>120</v>
       </c>
       <c r="AG183" s="1">
@@ -12174,7 +12294,7 @@
         <v>185</v>
       </c>
       <c r="Y184" s="3">
-        <f>N105</f>
+        <f t="shared" si="14"/>
         <v>103</v>
       </c>
       <c r="Z184" s="1">
@@ -12185,7 +12305,7 @@
         <v>182</v>
       </c>
       <c r="AF184" s="3">
-        <f>N123</f>
+        <f t="shared" si="15"/>
         <v>121</v>
       </c>
       <c r="AG184" s="1">
@@ -12198,7 +12318,7 @@
         <v>186</v>
       </c>
       <c r="Y185" s="3">
-        <f>N106</f>
+        <f t="shared" si="14"/>
         <v>104</v>
       </c>
       <c r="Z185" s="1">
@@ -12209,7 +12329,7 @@
         <v>183</v>
       </c>
       <c r="AF185" s="3">
-        <f>N124</f>
+        <f t="shared" si="15"/>
         <v>122</v>
       </c>
       <c r="AG185" s="1">
@@ -12222,7 +12342,7 @@
         <v>187</v>
       </c>
       <c r="Y186" s="3">
-        <f>N107</f>
+        <f t="shared" si="14"/>
         <v>105</v>
       </c>
       <c r="Z186" s="1">
@@ -12233,7 +12353,7 @@
         <v>184</v>
       </c>
       <c r="AF186" s="3">
-        <f>N125</f>
+        <f t="shared" si="15"/>
         <v>123</v>
       </c>
       <c r="AG186" s="1">
@@ -12246,7 +12366,7 @@
         <v>188</v>
       </c>
       <c r="Y187" s="3">
-        <f>N108</f>
+        <f t="shared" si="14"/>
         <v>106</v>
       </c>
       <c r="Z187" s="1">
@@ -12257,7 +12377,7 @@
         <v>185</v>
       </c>
       <c r="AF187" s="3">
-        <f>N126</f>
+        <f t="shared" si="15"/>
         <v>124</v>
       </c>
       <c r="AG187" s="1">
@@ -12270,7 +12390,7 @@
         <v>189</v>
       </c>
       <c r="Y188" s="3">
-        <f>N109</f>
+        <f t="shared" si="14"/>
         <v>107</v>
       </c>
       <c r="Z188" s="1">
@@ -12281,7 +12401,7 @@
         <v>186</v>
       </c>
       <c r="AF188" s="3">
-        <f>N127</f>
+        <f t="shared" si="15"/>
         <v>125</v>
       </c>
       <c r="AG188" s="1">
@@ -12294,7 +12414,7 @@
         <v>190</v>
       </c>
       <c r="Y189" s="3">
-        <f>N110</f>
+        <f t="shared" si="14"/>
         <v>108</v>
       </c>
       <c r="Z189" s="1">
@@ -12305,7 +12425,7 @@
         <v>187</v>
       </c>
       <c r="AF189" s="3">
-        <f>N128</f>
+        <f t="shared" si="15"/>
         <v>126</v>
       </c>
       <c r="AG189" s="1">
@@ -12335,7 +12455,7 @@
         <v>188</v>
       </c>
       <c r="AF190" s="3">
-        <f>N129</f>
+        <f t="shared" si="15"/>
         <v>127</v>
       </c>
       <c r="AG190" s="1">
@@ -12359,7 +12479,7 @@
         <v>189</v>
       </c>
       <c r="AF191" s="3">
-        <f>N130</f>
+        <f t="shared" si="15"/>
         <v>128</v>
       </c>
       <c r="AG191" s="1">
@@ -12383,7 +12503,7 @@
         <v>190</v>
       </c>
       <c r="AF192" s="3">
-        <f>N131</f>
+        <f t="shared" si="15"/>
         <v>129</v>
       </c>
       <c r="AG192" s="1">
@@ -12407,7 +12527,7 @@
         <v>191</v>
       </c>
       <c r="AF193" s="3">
-        <f>N132</f>
+        <f t="shared" si="15"/>
         <v>130</v>
       </c>
       <c r="AG193" s="1">
@@ -12420,7 +12540,7 @@
         <v>195</v>
       </c>
       <c r="Y194" s="3">
-        <f>N111</f>
+        <f t="shared" ref="Y194:Y221" si="16">N111</f>
         <v>109</v>
       </c>
       <c r="Z194" s="1">
@@ -12431,7 +12551,7 @@
         <v>192</v>
       </c>
       <c r="AF194" s="3">
-        <f>N133</f>
+        <f t="shared" si="15"/>
         <v>131</v>
       </c>
       <c r="AG194" s="1">
@@ -12444,7 +12564,7 @@
         <v>196</v>
       </c>
       <c r="Y195" s="3">
-        <f>N112</f>
+        <f t="shared" si="16"/>
         <v>110</v>
       </c>
       <c r="Z195" s="1">
@@ -12455,7 +12575,7 @@
         <v>193</v>
       </c>
       <c r="AF195" s="3">
-        <f>N134</f>
+        <f t="shared" si="15"/>
         <v>132</v>
       </c>
       <c r="AG195" s="1">
@@ -12468,7 +12588,7 @@
         <v>197</v>
       </c>
       <c r="Y196" s="3">
-        <f>N113</f>
+        <f t="shared" si="16"/>
         <v>111</v>
       </c>
       <c r="Z196" s="1">
@@ -12479,7 +12599,7 @@
         <v>194</v>
       </c>
       <c r="AF196" s="3">
-        <f>N135</f>
+        <f t="shared" si="15"/>
         <v>133</v>
       </c>
       <c r="AG196" s="1">
@@ -12492,7 +12612,7 @@
         <v>198</v>
       </c>
       <c r="Y197" s="3">
-        <f>N114</f>
+        <f t="shared" si="16"/>
         <v>112</v>
       </c>
       <c r="Z197" s="1">
@@ -12503,7 +12623,7 @@
         <v>195</v>
       </c>
       <c r="AF197" s="3">
-        <f>N136</f>
+        <f t="shared" si="15"/>
         <v>134</v>
       </c>
       <c r="AG197" s="1">
@@ -12516,7 +12636,7 @@
         <v>199</v>
       </c>
       <c r="Y198" s="3">
-        <f>N115</f>
+        <f t="shared" si="16"/>
         <v>113</v>
       </c>
       <c r="Z198" s="1">
@@ -12527,7 +12647,7 @@
         <v>196</v>
       </c>
       <c r="AF198" s="3">
-        <f>N137</f>
+        <f t="shared" si="15"/>
         <v>135</v>
       </c>
       <c r="AG198" s="1">
@@ -12540,7 +12660,7 @@
         <v>200</v>
       </c>
       <c r="Y199" s="3">
-        <f>N116</f>
+        <f t="shared" si="16"/>
         <v>114</v>
       </c>
       <c r="Z199" s="1">
@@ -12551,7 +12671,7 @@
         <v>197</v>
       </c>
       <c r="AF199" s="3">
-        <f>N138</f>
+        <f t="shared" si="15"/>
         <v>136</v>
       </c>
       <c r="AG199" s="1">
@@ -12564,7 +12684,7 @@
         <v>201</v>
       </c>
       <c r="Y200" s="3">
-        <f>N117</f>
+        <f t="shared" si="16"/>
         <v>115</v>
       </c>
       <c r="Z200" s="1">
@@ -12575,7 +12695,7 @@
         <v>198</v>
       </c>
       <c r="AF200" s="3">
-        <f>N139</f>
+        <f t="shared" si="15"/>
         <v>137</v>
       </c>
       <c r="AG200" s="1">
@@ -12588,7 +12708,7 @@
         <v>202</v>
       </c>
       <c r="Y201" s="3">
-        <f>N118</f>
+        <f t="shared" si="16"/>
         <v>116</v>
       </c>
       <c r="Z201" s="1">
@@ -12599,7 +12719,7 @@
         <v>199</v>
       </c>
       <c r="AF201" s="3">
-        <f>N140</f>
+        <f t="shared" si="15"/>
         <v>138</v>
       </c>
       <c r="AG201" s="1">
@@ -12612,7 +12732,7 @@
         <v>203</v>
       </c>
       <c r="Y202" s="3">
-        <f>N119</f>
+        <f t="shared" si="16"/>
         <v>117</v>
       </c>
       <c r="Z202" s="1">
@@ -12623,7 +12743,7 @@
         <v>200</v>
       </c>
       <c r="AF202" s="3">
-        <f>N131</f>
+        <f t="shared" ref="AF202:AF211" si="17">N131</f>
         <v>129</v>
       </c>
       <c r="AG202" s="1">
@@ -12636,7 +12756,7 @@
         <v>204</v>
       </c>
       <c r="Y203" s="3">
-        <f>N120</f>
+        <f t="shared" si="16"/>
         <v>118</v>
       </c>
       <c r="Z203" s="1">
@@ -12647,7 +12767,7 @@
         <v>201</v>
       </c>
       <c r="AF203" s="3">
-        <f>N132</f>
+        <f t="shared" si="17"/>
         <v>130</v>
       </c>
       <c r="AG203" s="1">
@@ -12660,7 +12780,7 @@
         <v>205</v>
       </c>
       <c r="Y204" s="3">
-        <f>N121</f>
+        <f t="shared" si="16"/>
         <v>119</v>
       </c>
       <c r="Z204" s="1">
@@ -12671,7 +12791,7 @@
         <v>202</v>
       </c>
       <c r="AF204" s="3">
-        <f>N133</f>
+        <f t="shared" si="17"/>
         <v>131</v>
       </c>
       <c r="AG204" s="1">
@@ -12684,7 +12804,7 @@
         <v>206</v>
       </c>
       <c r="Y205" s="3">
-        <f>N122</f>
+        <f t="shared" si="16"/>
         <v>120</v>
       </c>
       <c r="Z205" s="1">
@@ -12695,7 +12815,7 @@
         <v>203</v>
       </c>
       <c r="AF205" s="3">
-        <f>N134</f>
+        <f t="shared" si="17"/>
         <v>132</v>
       </c>
       <c r="AG205" s="1">
@@ -12708,7 +12828,7 @@
         <v>207</v>
       </c>
       <c r="Y206" s="3">
-        <f>N123</f>
+        <f t="shared" si="16"/>
         <v>121</v>
       </c>
       <c r="Z206" s="1">
@@ -12719,7 +12839,7 @@
         <v>204</v>
       </c>
       <c r="AF206" s="3">
-        <f>N135</f>
+        <f t="shared" si="17"/>
         <v>133</v>
       </c>
       <c r="AG206" s="1">
@@ -12735,7 +12855,7 @@
         <v>208</v>
       </c>
       <c r="Y207" s="3">
-        <f>N124</f>
+        <f t="shared" si="16"/>
         <v>122</v>
       </c>
       <c r="Z207" s="1">
@@ -12746,7 +12866,7 @@
         <v>205</v>
       </c>
       <c r="AF207" s="3">
-        <f>N136</f>
+        <f t="shared" si="17"/>
         <v>134</v>
       </c>
       <c r="AG207" s="1">
@@ -12762,7 +12882,7 @@
         <v>209</v>
       </c>
       <c r="Y208" s="3">
-        <f>N125</f>
+        <f t="shared" si="16"/>
         <v>123</v>
       </c>
       <c r="Z208" s="1">
@@ -12773,7 +12893,7 @@
         <v>206</v>
       </c>
       <c r="AF208" s="3">
-        <f>N137</f>
+        <f t="shared" si="17"/>
         <v>135</v>
       </c>
       <c r="AG208" s="1">
@@ -12789,7 +12909,7 @@
         <v>210</v>
       </c>
       <c r="Y209" s="3">
-        <f>N126</f>
+        <f t="shared" si="16"/>
         <v>124</v>
       </c>
       <c r="Z209" s="1">
@@ -12800,7 +12920,7 @@
         <v>207</v>
       </c>
       <c r="AF209" s="3">
-        <f>N138</f>
+        <f t="shared" si="17"/>
         <v>136</v>
       </c>
       <c r="AG209" s="1">
@@ -12816,7 +12936,7 @@
         <v>211</v>
       </c>
       <c r="Y210" s="3">
-        <f>N127</f>
+        <f t="shared" si="16"/>
         <v>125</v>
       </c>
       <c r="Z210" s="1">
@@ -12827,7 +12947,7 @@
         <v>208</v>
       </c>
       <c r="AF210" s="3">
-        <f>N139</f>
+        <f t="shared" si="17"/>
         <v>137</v>
       </c>
       <c r="AG210" s="1">
@@ -12843,7 +12963,7 @@
         <v>212</v>
       </c>
       <c r="Y211" s="3">
-        <f>N128</f>
+        <f t="shared" si="16"/>
         <v>126</v>
       </c>
       <c r="Z211" s="1">
@@ -12854,7 +12974,7 @@
         <v>209</v>
       </c>
       <c r="AF211" s="3">
-        <f>N140</f>
+        <f t="shared" si="17"/>
         <v>138</v>
       </c>
       <c r="AG211" s="1">
@@ -12870,7 +12990,7 @@
         <v>213</v>
       </c>
       <c r="Y212" s="3">
-        <f>N129</f>
+        <f t="shared" si="16"/>
         <v>127</v>
       </c>
       <c r="Z212" s="1">
@@ -12886,7 +13006,7 @@
         <v>214</v>
       </c>
       <c r="Y213" s="3">
-        <f>N130</f>
+        <f t="shared" si="16"/>
         <v>128</v>
       </c>
       <c r="Z213" s="1">
@@ -12902,7 +13022,7 @@
         <v>215</v>
       </c>
       <c r="Y214" s="3">
-        <f>N131</f>
+        <f t="shared" si="16"/>
         <v>129</v>
       </c>
       <c r="Z214" s="1">
@@ -12918,7 +13038,7 @@
         <v>216</v>
       </c>
       <c r="Y215" s="3">
-        <f>N132</f>
+        <f t="shared" si="16"/>
         <v>130</v>
       </c>
       <c r="Z215" s="1">
@@ -12934,7 +13054,7 @@
         <v>217</v>
       </c>
       <c r="Y216" s="3">
-        <f>N133</f>
+        <f t="shared" si="16"/>
         <v>131</v>
       </c>
       <c r="Z216" s="1">
@@ -12951,7 +13071,7 @@
         <v>218</v>
       </c>
       <c r="Y217" s="3">
-        <f>N134</f>
+        <f t="shared" si="16"/>
         <v>132</v>
       </c>
       <c r="Z217" s="1">
@@ -12968,7 +13088,7 @@
         <v>219</v>
       </c>
       <c r="Y218" s="3">
-        <f>N135</f>
+        <f t="shared" si="16"/>
         <v>133</v>
       </c>
       <c r="Z218" s="1">
@@ -12985,7 +13105,7 @@
         <v>220</v>
       </c>
       <c r="Y219" s="3">
-        <f>N136</f>
+        <f t="shared" si="16"/>
         <v>134</v>
       </c>
       <c r="Z219" s="1">
@@ -13002,7 +13122,7 @@
         <v>221</v>
       </c>
       <c r="Y220" s="3">
-        <f>N137</f>
+        <f t="shared" si="16"/>
         <v>135</v>
       </c>
       <c r="Z220" s="1">
@@ -13019,7 +13139,7 @@
         <v>222</v>
       </c>
       <c r="Y221" s="3">
-        <f>N138</f>
+        <f t="shared" si="16"/>
         <v>136</v>
       </c>
       <c r="Z221" s="1">
@@ -13135,13 +13255,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AW1:AY1"/>
-    <mergeCell ref="AZ1:BB1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AN1:AP1"/>
-    <mergeCell ref="AQ1:AS1"/>
-    <mergeCell ref="AT1:AV1"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="AA1:AD1"/>
@@ -13150,6 +13263,13 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="S1:W1"/>
+    <mergeCell ref="AW1:AY1"/>
+    <mergeCell ref="AZ1:BB1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="AN1:AP1"/>
+    <mergeCell ref="AQ1:AS1"/>
+    <mergeCell ref="AT1:AV1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>